<commit_message>
Frist XGBoost model and CV
</commit_message>
<xml_diff>
--- a/3.feature_ranking/feature_ranking.xlsx
+++ b/3.feature_ranking/feature_ranking.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.0005654550879112819</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01334267371368014</v>
+        <v>0.0152987983553583</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.07478795000303506</v>
+        <v>0.07207341979134174</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04538964670152801</v>
+        <v>0.04425037842602819</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.004303959438815674</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.006024484544363773</v>
+        <v>0.0003203212830724667</v>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.004936149597882356</v>
+        <v>0.003147217299551031</v>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -556,10 +556,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.00231072907423524</v>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -569,10 +569,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.00207724329404968</v>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -582,10 +582,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.001036879735875296</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
@@ -608,10 +608,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.0004063500479780657</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02200848112771769</v>
+        <v>0.02258330274355114</v>
       </c>
       <c r="C16" t="n">
         <v>7</v>
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.00991533171148351</v>
+        <v>0.006922060751502812</v>
       </c>
       <c r="C18" t="n">
         <v>5</v>
@@ -673,10 +673,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0102566184789632</v>
+        <v>0.00700913032577688</v>
       </c>
       <c r="C19" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.004257826738818693</v>
+        <v>0.01043456322946934</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.001111904599320646</v>
+        <v>0.001829928053239449</v>
       </c>
       <c r="C21" t="n">
         <v>8</v>
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.006217278124383441</v>
+        <v>0.001297756900458857</v>
       </c>
       <c r="C22" t="n">
         <v>8</v>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.01950421414320314</v>
+        <v>0.02028643846604705</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.04169924435889882</v>
+        <v>0.04050943981025679</v>
       </c>
       <c r="C24" t="n">
         <v>12</v>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04018492337554935</v>
+        <v>0.03647524836086635</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.04637331978514769</v>
+        <v>0.04684119439717893</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.04595340041838369</v>
+        <v>0.04636743495132034</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.05673451048683376</v>
+        <v>0.05639383736517622</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.05852908364726694</v>
+        <v>0.05666897832244366</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.05266329292998595</v>
+        <v>0.05261479791126966</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.06242836393814155</v>
+        <v>0.06167280379676754</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.06383155218259695</v>
+        <v>0.06226873842624325</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.007879834094015159</v>
+        <v>0.008303656323646713</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
@@ -868,7 +868,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.00939146100456334</v>
+        <v>0.007256950239384885</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
@@ -881,7 +881,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.01501807721804749</v>
+        <v>0.01163556754276041</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01022781990795085</v>
+        <v>0.008569525125595057</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.01151664225370297</v>
+        <v>0.01518035013359142</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.01637521679830645</v>
+        <v>0.01345291701184426</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>

</xml_diff>